<commit_message>
feat: Split the pm-study-plan table.
</commit_message>
<xml_diff>
--- a/___/table/pm-study-plan/长期学习PM计划.xlsx
+++ b/___/table/pm-study-plan/长期学习PM计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13300" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="30240" windowHeight="13640" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PMP认证课" sheetId="1" r:id="rId1"/>
@@ -49,13 +49,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="177" formatCode="mmm\ dd"/>
+    <numFmt numFmtId="176" formatCode="mmm\ dd"/>
+    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="ddd"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -151,6 +151,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -164,22 +171,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -188,8 +179,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,6 +192,13 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -220,52 +219,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,11 +240,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -321,19 +321,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +345,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,31 +405,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,19 +435,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,67 +447,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +471,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,8 +512,28 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,15 +553,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -552,6 +563,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -574,35 +600,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,148 +611,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -762,10 +762,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,10 +810,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,7 +1098,7 @@
                 <a:latin typeface="黑体" charset="0"/>
                 <a:ea typeface="黑体" charset="0"/>
               </a:rPr>
-              <a:t>先导课计划任务管理表</a:t>
+              <a:t>PMP认证课计划任务管理表</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
               <a:solidFill>
@@ -1319,7 +1319,7 @@
                 <a:latin typeface="黑体" charset="0"/>
                 <a:ea typeface="黑体" charset="0"/>
               </a:rPr>
-              <a:t>词汇课计划任务管理表</a:t>
+              <a:t>ACP认证课计划任务管理表</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
               <a:solidFill>
@@ -1533,16 +1533,16 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1">
                 <a:solidFill>
                   <a:srgbClr val="333333"/>
                 </a:solidFill>
                 <a:latin typeface="黑体" charset="0"/>
                 <a:ea typeface="黑体" charset="0"/>
               </a:rPr>
-              <a:t>阅读课计划任务管理表</a:t>
+              <a:t>信息系统项目管理师计划任务管理表</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="2400" b="1">
               <a:solidFill>
                 <a:srgbClr val="333333"/>
               </a:solidFill>
@@ -1754,16 +1754,16 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2000" b="1">
                 <a:solidFill>
                   <a:srgbClr val="333333"/>
                 </a:solidFill>
                 <a:latin typeface="黑体" charset="0"/>
                 <a:ea typeface="黑体" charset="0"/>
               </a:rPr>
-              <a:t>听口课计划任务管理表</a:t>
+              <a:t>项目管理实战Plus精英班计划任务管理表</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="2000" b="1">
               <a:solidFill>
                 <a:srgbClr val="333333"/>
               </a:solidFill>
@@ -1811,15 +1811,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>407467</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>126541</xdr:rowOff>
+      <xdr:colOff>407035</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>8255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>829977</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>164715</xdr:rowOff>
+      <xdr:colOff>850900</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1828,10 +1828,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="722630" y="307340"/>
-          <a:ext cx="5891530" cy="581025"/>
-          <a:chOff x="735420" y="454122"/>
-          <a:chExt cx="5131980" cy="869633"/>
+          <a:off x="722630" y="370205"/>
+          <a:ext cx="5912485" cy="582295"/>
+          <a:chOff x="735420" y="549686"/>
+          <a:chExt cx="5150744" cy="869633"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -1841,7 +1841,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1302786" y="454122"/>
+            <a:off x="1321550" y="549686"/>
             <a:ext cx="4564614" cy="869633"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -1975,16 +1975,16 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
                 <a:solidFill>
                   <a:srgbClr val="333333"/>
                 </a:solidFill>
                 <a:latin typeface="黑体" charset="0"/>
                 <a:ea typeface="黑体" charset="0"/>
               </a:rPr>
-              <a:t>翻译课计划任务管理表</a:t>
+              <a:t>产品经理核心能力入门必修课计划任务管理表</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
               <a:solidFill>
                 <a:srgbClr val="333333"/>
               </a:solidFill>
@@ -2196,16 +2196,16 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1">
                 <a:solidFill>
                   <a:srgbClr val="333333"/>
                 </a:solidFill>
                 <a:latin typeface="黑体" charset="0"/>
                 <a:ea typeface="黑体" charset="0"/>
               </a:rPr>
-              <a:t>PET3级计划任务管理表</a:t>
+              <a:t>产品总监冲刺班计划任务管理表</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="3200" b="1">
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="2400" b="1">
               <a:solidFill>
                 <a:srgbClr val="333333"/>
               </a:solidFill>
@@ -5560,7 +5560,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{421099d4-1bc6-4a4d-80d9-e5b1e6d2abb4}</x14:id>
+          <x14:id>{62ef874b-1280-45fd-beca-e54aba79298a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5572,7 +5572,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bf5fed55-fda2-41aa-9eb6-e1af4c759a53}</x14:id>
+          <x14:id>{7a7cb098-7c21-49d2-9629-b86f66b9506e}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5589,7 +5589,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{421099d4-1bc6-4a4d-80d9-e5b1e6d2abb4}">
+          <x14:cfRule type="dataBar" id="{62ef874b-1280-45fd-beca-e54aba79298a}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -5600,7 +5600,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{bf5fed55-fda2-41aa-9eb6-e1af4c759a53}">
+          <x14:cfRule type="dataBar" id="{7a7cb098-7c21-49d2-9629-b86f66b9506e}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8455,7 +8455,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{66143e1f-080a-4541-82c3-cae4d772f58d}</x14:id>
+          <x14:id>{e172d228-c170-4d77-a561-5b2ccd61f153}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8467,7 +8467,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4d35040d-b1a6-4a77-a1f0-8c6b5cd23319}</x14:id>
+          <x14:id>{7b26c761-8a07-4a74-a823-7ff2e67c9a31}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8484,7 +8484,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{66143e1f-080a-4541-82c3-cae4d772f58d}">
+          <x14:cfRule type="dataBar" id="{e172d228-c170-4d77-a561-5b2ccd61f153}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8495,7 +8495,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{4d35040d-b1a6-4a77-a1f0-8c6b5cd23319}">
+          <x14:cfRule type="dataBar" id="{7b26c761-8a07-4a74-a823-7ff2e67c9a31}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8520,7 +8520,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="12.8"/>
@@ -11350,7 +11350,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c28d4e19-688b-46e8-9b57-97ae8817543b}</x14:id>
+          <x14:id>{2902651d-d070-43a8-8f2f-86b8f454372c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11362,7 +11362,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0c1fd25c-1cec-4f39-b41a-c34a652dcf3d}</x14:id>
+          <x14:id>{ad536c51-65ca-4c94-9d72-ef074e003d5e}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11379,7 +11379,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c28d4e19-688b-46e8-9b57-97ae8817543b}">
+          <x14:cfRule type="dataBar" id="{2902651d-d070-43a8-8f2f-86b8f454372c}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11390,7 +11390,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{0c1fd25c-1cec-4f39-b41a-c34a652dcf3d}">
+          <x14:cfRule type="dataBar" id="{ad536c51-65ca-4c94-9d72-ef074e003d5e}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11415,7 +11415,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="12.8"/>
@@ -14245,7 +14245,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bce11c0d-7f58-4954-a533-ec9dd715f7e6}</x14:id>
+          <x14:id>{8e78fd62-c3e6-4cce-977e-8524d2317855}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -14257,7 +14257,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{66592114-c888-40f8-b448-8374ccce011e}</x14:id>
+          <x14:id>{3bb0b3b5-d01d-48af-8e0c-01d7e6936915}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -14274,7 +14274,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bce11c0d-7f58-4954-a533-ec9dd715f7e6}">
+          <x14:cfRule type="dataBar" id="{8e78fd62-c3e6-4cce-977e-8524d2317855}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -14285,7 +14285,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{66592114-c888-40f8-b448-8374ccce011e}">
+          <x14:cfRule type="dataBar" id="{3bb0b3b5-d01d-48af-8e0c-01d7e6936915}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -14310,7 +14310,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="12.8"/>
@@ -17140,7 +17140,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c317df35-d0bf-4636-b332-bd3b379ad111}</x14:id>
+          <x14:id>{1adc383f-a547-40f1-a084-600de2e4fe5a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -17152,7 +17152,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3b7e68c2-72b2-4ad7-94d3-d1a1b36a1149}</x14:id>
+          <x14:id>{aaa2bca3-f481-4a94-84d3-972016de6877}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -17169,7 +17169,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c317df35-d0bf-4636-b332-bd3b379ad111}">
+          <x14:cfRule type="dataBar" id="{1adc383f-a547-40f1-a084-600de2e4fe5a}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -17180,7 +17180,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{3b7e68c2-72b2-4ad7-94d3-d1a1b36a1149}">
+          <x14:cfRule type="dataBar" id="{aaa2bca3-f481-4a94-84d3-972016de6877}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -17205,7 +17205,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="12.8"/>
@@ -20035,7 +20035,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8fe2d1e6-82ae-4ea1-9ac4-4ac1fbaa52d5}</x14:id>
+          <x14:id>{b0e45986-3355-44fe-abee-68107ff5721d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -20047,7 +20047,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e10140e7-fe71-4c3e-aea3-282c0d34e4f0}</x14:id>
+          <x14:id>{3e10b62a-d26d-4e95-b563-55d3e6932f08}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -20064,7 +20064,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8fe2d1e6-82ae-4ea1-9ac4-4ac1fbaa52d5}">
+          <x14:cfRule type="dataBar" id="{b0e45986-3355-44fe-abee-68107ff5721d}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -20075,7 +20075,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{e10140e7-fe71-4c3e-aea3-282c0d34e4f0}">
+          <x14:cfRule type="dataBar" id="{3e10b62a-d26d-4e95-b563-55d3e6932f08}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -20100,7 +20100,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="12.8"/>
@@ -22930,7 +22930,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c9658a2b-9ce0-43e8-a4b6-4b60525c3774}</x14:id>
+          <x14:id>{09d16e98-d2ef-481f-ad3a-60e40846845c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22942,7 +22942,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{308e33c4-3604-43fd-bd29-ad79f17f1d98}</x14:id>
+          <x14:id>{03c1570d-fa03-4c03-81bd-36b88cd12d55}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22959,7 +22959,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c9658a2b-9ce0-43e8-a4b6-4b60525c3774}">
+          <x14:cfRule type="dataBar" id="{09d16e98-d2ef-481f-ad3a-60e40846845c}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -22970,7 +22970,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{308e33c4-3604-43fd-bd29-ad79f17f1d98}">
+          <x14:cfRule type="dataBar" id="{03c1570d-fa03-4c03-81bd-36b88cd12d55}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>